<commit_message>
working on seeral bugs, need refactoring
</commit_message>
<xml_diff>
--- a/Leerplanillacupos/data/020823.xlsx
+++ b/Leerplanillacupos/data/020823.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fi365.sharepoint.com/sites/CoordinacinctedraISCovit-19-CoordinacinMateriasCarreras/Documentos compartidos/Coordinación Materias Carreras/PlanificacionSemestres/2023/Sem 2/Inscripciones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gastonmousques/workspace/IngSoftTools/excelconverter/Leerplanillacupos/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{88BF50D7-32FE-401C-8DEC-49E1B5B46623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D153FEE1-208C-984D-8A62-8EA8EB3BBB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1200" windowWidth="23115" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="1200" windowWidth="23120" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TDICTADO.RPT" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="517">
   <si>
     <t>Listado Tabular de Dictados</t>
   </si>
@@ -1584,6 +1584,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Web mining</t>
+  </si>
+  <si>
+    <t>Materia</t>
   </si>
 </sst>
 </file>
@@ -1601,27 +1604,32 @@
       <sz val="14.05"/>
       <color indexed="8"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8.9"/>
       <color indexed="8"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9.85"/>
       <color indexed="8"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8.9"/>
       <color indexed="8"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8.15"/>
       <color indexed="8"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1732,9 +1740,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1772,7 +1780,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1878,7 +1886,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2020,7 +2028,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2031,16 +2039,16 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:G271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F145" sqref="F145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18">
@@ -2048,14 +2056,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.5">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>516</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2067,7 +2077,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" hidden="1"/>
-    <row r="8" spans="1:7" ht="13.5" hidden="1">
+    <row r="8" spans="1:7" ht="14" hidden="1">
       <c r="A8" s="7">
         <v>66433</v>
       </c>
@@ -2090,7 +2100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.5" hidden="1">
+    <row r="9" spans="1:7" ht="14" hidden="1">
       <c r="A9" s="7">
         <v>66077</v>
       </c>
@@ -2113,7 +2123,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13.5" hidden="1">
+    <row r="10" spans="1:7" ht="14" hidden="1">
       <c r="A10" s="7">
         <v>66095</v>
       </c>
@@ -2136,7 +2146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="13.5" hidden="1">
+    <row r="11" spans="1:7" ht="14" hidden="1">
       <c r="A11" s="7">
         <v>66464</v>
       </c>
@@ -2159,7 +2169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13.5" hidden="1">
+    <row r="12" spans="1:7" ht="14" hidden="1">
       <c r="A12" s="7">
         <v>66465</v>
       </c>
@@ -2182,7 +2192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="13.5">
+    <row r="13" spans="1:7" ht="14">
       <c r="A13" s="7">
         <v>66442</v>
       </c>
@@ -2205,7 +2215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="13.5">
+    <row r="14" spans="1:7" ht="14">
       <c r="A14" s="7">
         <v>66440</v>
       </c>
@@ -2228,7 +2238,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.5" hidden="1">
+    <row r="15" spans="1:7" ht="14" hidden="1">
       <c r="A15" s="7">
         <v>66368</v>
       </c>
@@ -2251,7 +2261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13.5" hidden="1">
+    <row r="16" spans="1:7" ht="14" hidden="1">
       <c r="A16" s="7">
         <v>66369</v>
       </c>
@@ -2274,7 +2284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="13.5" hidden="1">
+    <row r="17" spans="1:7" ht="14" hidden="1">
       <c r="A17" s="7">
         <v>66367</v>
       </c>
@@ -2297,7 +2307,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13.5">
+    <row r="18" spans="1:7" ht="14">
       <c r="A18" s="7">
         <v>66515</v>
       </c>
@@ -2320,7 +2330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.5" hidden="1">
+    <row r="19" spans="1:7" ht="14" hidden="1">
       <c r="A19" s="7">
         <v>66469</v>
       </c>
@@ -2343,7 +2353,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.5">
+    <row r="20" spans="1:7" ht="14">
       <c r="A20" s="7">
         <v>66758</v>
       </c>
@@ -2366,7 +2376,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13.5" hidden="1">
+    <row r="21" spans="1:7" ht="14" hidden="1">
       <c r="A21" s="7">
         <v>66055</v>
       </c>
@@ -2389,7 +2399,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.5" hidden="1">
+    <row r="22" spans="1:7" ht="14" hidden="1">
       <c r="A22" s="7">
         <v>66043</v>
       </c>
@@ -2412,7 +2422,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13.5" hidden="1">
+    <row r="23" spans="1:7" ht="14" hidden="1">
       <c r="A23" s="7">
         <v>66049</v>
       </c>
@@ -2435,7 +2445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13.5" hidden="1">
+    <row r="24" spans="1:7" ht="14" hidden="1">
       <c r="A24" s="7">
         <v>66439</v>
       </c>
@@ -2458,7 +2468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.5" hidden="1">
+    <row r="25" spans="1:7" ht="14" hidden="1">
       <c r="A25" s="7">
         <v>66283</v>
       </c>
@@ -2481,7 +2491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="13.5" hidden="1">
+    <row r="26" spans="1:7" ht="14" hidden="1">
       <c r="A26" s="7">
         <v>66424</v>
       </c>
@@ -2504,7 +2514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.5" hidden="1">
+    <row r="27" spans="1:7" ht="14" hidden="1">
       <c r="A27" s="7">
         <v>66425</v>
       </c>
@@ -2527,7 +2537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13.5" hidden="1">
+    <row r="28" spans="1:7" ht="14" hidden="1">
       <c r="A28" s="7">
         <v>66279</v>
       </c>
@@ -2550,7 +2560,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.5" hidden="1">
+    <row r="29" spans="1:7" ht="14" hidden="1">
       <c r="A29" s="7">
         <v>66421</v>
       </c>
@@ -2573,7 +2583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="13.5" hidden="1">
+    <row r="30" spans="1:7" ht="14" hidden="1">
       <c r="A30" s="7">
         <v>66422</v>
       </c>
@@ -2596,7 +2606,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="13.5" hidden="1">
+    <row r="31" spans="1:7" ht="14" hidden="1">
       <c r="A31" s="7">
         <v>66423</v>
       </c>
@@ -2619,7 +2629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.5" hidden="1">
+    <row r="32" spans="1:7" ht="14" hidden="1">
       <c r="A32" s="7">
         <v>66282</v>
       </c>
@@ -2642,7 +2652,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.5" hidden="1">
+    <row r="33" spans="1:7" ht="14" hidden="1">
       <c r="A33" s="7">
         <v>66429</v>
       </c>
@@ -2665,7 +2675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.5" hidden="1">
+    <row r="34" spans="1:7" ht="14" hidden="1">
       <c r="A34" s="7">
         <v>66289</v>
       </c>
@@ -2688,7 +2698,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="13.5" hidden="1">
+    <row r="35" spans="1:7" ht="14" hidden="1">
       <c r="A35" s="7">
         <v>66293</v>
       </c>
@@ -2711,7 +2721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="13.5" hidden="1">
+    <row r="36" spans="1:7" ht="14" hidden="1">
       <c r="A36" s="7">
         <v>66292</v>
       </c>
@@ -2734,7 +2744,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="13.5" hidden="1">
+    <row r="37" spans="1:7" ht="14" hidden="1">
       <c r="A37" s="7">
         <v>66427</v>
       </c>
@@ -2757,7 +2767,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="13.5" hidden="1">
+    <row r="38" spans="1:7" ht="14" hidden="1">
       <c r="A38" s="7">
         <v>66438</v>
       </c>
@@ -2780,7 +2790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="13.5" hidden="1">
+    <row r="39" spans="1:7" ht="14" hidden="1">
       <c r="A39" s="7">
         <v>66301</v>
       </c>
@@ -2803,7 +2813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="13.5" hidden="1">
+    <row r="40" spans="1:7" ht="14" hidden="1">
       <c r="A40" s="7">
         <v>66089</v>
       </c>
@@ -2826,7 +2836,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="13.5" hidden="1">
+    <row r="41" spans="1:7" ht="14" hidden="1">
       <c r="A41" s="7">
         <v>66079</v>
       </c>
@@ -2849,7 +2859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="13.5" hidden="1">
+    <row r="42" spans="1:7" ht="14" hidden="1">
       <c r="A42" s="7">
         <v>66066</v>
       </c>
@@ -2872,7 +2882,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="13.5" hidden="1">
+    <row r="43" spans="1:7" ht="14" hidden="1">
       <c r="A43" s="7">
         <v>66074</v>
       </c>
@@ -2895,7 +2905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.5" hidden="1">
+    <row r="44" spans="1:7" ht="14" hidden="1">
       <c r="A44" s="7">
         <v>66090</v>
       </c>
@@ -2918,7 +2928,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="13.5" hidden="1">
+    <row r="45" spans="1:7" ht="14" hidden="1">
       <c r="A45" s="7">
         <v>66080</v>
       </c>
@@ -2941,7 +2951,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13.5" hidden="1">
+    <row r="46" spans="1:7" ht="14" hidden="1">
       <c r="A46" s="7">
         <v>66092</v>
       </c>
@@ -2964,7 +2974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="13.5" hidden="1">
+    <row r="47" spans="1:7" ht="14" hidden="1">
       <c r="A47" s="7">
         <v>66084</v>
       </c>
@@ -2987,7 +2997,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="13.5" hidden="1">
+    <row r="48" spans="1:7" ht="14" hidden="1">
       <c r="A48" s="7">
         <v>66627</v>
       </c>
@@ -3010,7 +3020,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="13.5" hidden="1">
+    <row r="49" spans="1:7" ht="14" hidden="1">
       <c r="A49" s="7">
         <v>66632</v>
       </c>
@@ -3033,7 +3043,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="13.5" hidden="1">
+    <row r="50" spans="1:7" ht="14" hidden="1">
       <c r="A50" s="7">
         <v>66628</v>
       </c>
@@ -3056,7 +3066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="13.5" hidden="1">
+    <row r="51" spans="1:7" ht="14" hidden="1">
       <c r="A51" s="7">
         <v>66798</v>
       </c>
@@ -3079,7 +3089,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="13.5" hidden="1">
+    <row r="52" spans="1:7" ht="14" hidden="1">
       <c r="A52" s="7">
         <v>66527</v>
       </c>
@@ -3102,7 +3112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="13.5" hidden="1">
+    <row r="53" spans="1:7" ht="14" hidden="1">
       <c r="A53" s="7">
         <v>66523</v>
       </c>
@@ -3125,7 +3135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="13.5" hidden="1">
+    <row r="54" spans="1:7" ht="14" hidden="1">
       <c r="A54" s="7">
         <v>66468</v>
       </c>
@@ -3148,7 +3158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="13.5" hidden="1">
+    <row r="55" spans="1:7" ht="14" hidden="1">
       <c r="A55" s="7">
         <v>66445</v>
       </c>
@@ -3171,7 +3181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="13.5" hidden="1">
+    <row r="56" spans="1:7" ht="14" hidden="1">
       <c r="A56" s="7">
         <v>66444</v>
       </c>
@@ -3194,7 +3204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="13.5" hidden="1">
+    <row r="57" spans="1:7" ht="14" hidden="1">
       <c r="A57" s="7">
         <v>66759</v>
       </c>
@@ -3217,7 +3227,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="13.5" hidden="1">
+    <row r="58" spans="1:7" ht="14" hidden="1">
       <c r="A58" s="7">
         <v>66441</v>
       </c>
@@ -3240,7 +3250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="13.5">
+    <row r="59" spans="1:7" ht="14">
       <c r="A59" s="7">
         <v>66498</v>
       </c>
@@ -3263,7 +3273,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="13.5">
+    <row r="60" spans="1:7" ht="14">
       <c r="A60" s="7">
         <v>66454</v>
       </c>
@@ -3286,7 +3296,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="13.5">
+    <row r="61" spans="1:7" ht="14">
       <c r="A61" s="7">
         <v>66456</v>
       </c>
@@ -3309,7 +3319,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="13.5">
+    <row r="62" spans="1:7" ht="14">
       <c r="A62" s="7">
         <v>66459</v>
       </c>
@@ -3332,7 +3342,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="13.5">
+    <row r="63" spans="1:7" ht="14">
       <c r="A63" s="7">
         <v>66497</v>
       </c>
@@ -3355,7 +3365,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="13.5">
+    <row r="64" spans="1:7" ht="14">
       <c r="A64" s="7">
         <v>66460</v>
       </c>
@@ -3378,7 +3388,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="13.5">
+    <row r="65" spans="1:7" ht="14">
       <c r="A65" s="7">
         <v>66500</v>
       </c>
@@ -3401,7 +3411,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="13.5">
+    <row r="66" spans="1:7" ht="14">
       <c r="A66" s="7">
         <v>66501</v>
       </c>
@@ -3424,7 +3434,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="13.5">
+    <row r="67" spans="1:7" ht="14">
       <c r="A67" s="7">
         <v>66499</v>
       </c>
@@ -3447,7 +3457,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="13.5">
+    <row r="68" spans="1:7" ht="14">
       <c r="A68" s="7">
         <v>66461</v>
       </c>
@@ -3470,7 +3480,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="13.5">
+    <row r="69" spans="1:7" ht="14">
       <c r="A69" s="7">
         <v>66502</v>
       </c>
@@ -3493,7 +3503,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="13.5" hidden="1">
+    <row r="70" spans="1:7" ht="14" hidden="1">
       <c r="A70" s="7">
         <v>66631</v>
       </c>
@@ -3516,7 +3526,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="13.5" hidden="1">
+    <row r="71" spans="1:7" ht="14" hidden="1">
       <c r="A71" s="7">
         <v>66068</v>
       </c>
@@ -3539,7 +3549,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="13.5" hidden="1">
+    <row r="72" spans="1:7" ht="14" hidden="1">
       <c r="A72" s="7">
         <v>66076</v>
       </c>
@@ -3562,7 +3572,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="13.5" hidden="1">
+    <row r="73" spans="1:7" ht="14" hidden="1">
       <c r="A73" s="7">
         <v>66083</v>
       </c>
@@ -3585,7 +3595,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="13.5" hidden="1">
+    <row r="74" spans="1:7" ht="14" hidden="1">
       <c r="A74" s="7">
         <v>66648</v>
       </c>
@@ -3608,7 +3618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="13.5" hidden="1">
+    <row r="75" spans="1:7" ht="14" hidden="1">
       <c r="A75" s="7">
         <v>66642</v>
       </c>
@@ -3631,7 +3641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="13.5" hidden="1">
+    <row r="76" spans="1:7" ht="14" hidden="1">
       <c r="A76" s="7">
         <v>66646</v>
       </c>
@@ -3654,7 +3664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="13.5" hidden="1">
+    <row r="77" spans="1:7" ht="14" hidden="1">
       <c r="A77" s="7">
         <v>66311</v>
       </c>
@@ -3677,7 +3687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="13.5" hidden="1">
+    <row r="78" spans="1:7" ht="14" hidden="1">
       <c r="A78" s="7">
         <v>66316</v>
       </c>
@@ -3700,7 +3710,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="13.5" hidden="1">
+    <row r="79" spans="1:7" ht="14" hidden="1">
       <c r="A79" s="7">
         <v>66365</v>
       </c>
@@ -3723,7 +3733,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="13.5" hidden="1">
+    <row r="80" spans="1:7" ht="14" hidden="1">
       <c r="A80" s="7">
         <v>66364</v>
       </c>
@@ -3746,7 +3756,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="13.5" hidden="1">
+    <row r="81" spans="1:7" ht="14" hidden="1">
       <c r="A81" s="7">
         <v>66315</v>
       </c>
@@ -3769,7 +3779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="13.5" hidden="1">
+    <row r="82" spans="1:7" ht="14" hidden="1">
       <c r="A82" s="7">
         <v>66317</v>
       </c>
@@ -3792,7 +3802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="13.5" hidden="1">
+    <row r="83" spans="1:7" ht="14" hidden="1">
       <c r="A83" s="7">
         <v>66380</v>
       </c>
@@ -3815,7 +3825,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="13.5" hidden="1">
+    <row r="84" spans="1:7" ht="14" hidden="1">
       <c r="A84" s="7">
         <v>66377</v>
       </c>
@@ -3838,7 +3848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="13.5" hidden="1">
+    <row r="85" spans="1:7" ht="14" hidden="1">
       <c r="A85" s="7">
         <v>66378</v>
       </c>
@@ -3861,7 +3871,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="13.5" hidden="1">
+    <row r="86" spans="1:7" ht="14" hidden="1">
       <c r="A86" s="7">
         <v>66379</v>
       </c>
@@ -3884,7 +3894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="13.5" hidden="1">
+    <row r="87" spans="1:7" ht="14" hidden="1">
       <c r="A87" s="7">
         <v>66381</v>
       </c>
@@ -3907,7 +3917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="13.5" hidden="1">
+    <row r="88" spans="1:7" ht="14" hidden="1">
       <c r="A88" s="7">
         <v>66450</v>
       </c>
@@ -3930,7 +3940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="13.5" hidden="1">
+    <row r="89" spans="1:7" ht="14" hidden="1">
       <c r="A89" s="7">
         <v>66449</v>
       </c>
@@ -3953,7 +3963,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="13.5" hidden="1">
+    <row r="90" spans="1:7" ht="14" hidden="1">
       <c r="A90" s="7">
         <v>66309</v>
       </c>
@@ -3976,7 +3986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="13.5" hidden="1">
+    <row r="91" spans="1:7" ht="14" hidden="1">
       <c r="A91" s="7">
         <v>66056</v>
       </c>
@@ -3999,7 +4009,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="13.5" hidden="1">
+    <row r="92" spans="1:7" ht="14" hidden="1">
       <c r="A92" s="7">
         <v>66044</v>
       </c>
@@ -4022,7 +4032,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="13.5" hidden="1">
+    <row r="93" spans="1:7" ht="14" hidden="1">
       <c r="A93" s="7">
         <v>66050</v>
       </c>
@@ -4045,7 +4055,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="13.5" hidden="1">
+    <row r="94" spans="1:7" ht="14" hidden="1">
       <c r="A94" s="7">
         <v>66629</v>
       </c>
@@ -4068,7 +4078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="13.5" hidden="1">
+    <row r="95" spans="1:7" ht="14" hidden="1">
       <c r="A95" s="7">
         <v>66073</v>
       </c>
@@ -4091,7 +4101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="13.5" hidden="1">
+    <row r="96" spans="1:7" ht="14" hidden="1">
       <c r="A96" s="7">
         <v>66065</v>
       </c>
@@ -4114,7 +4124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="13.5" hidden="1">
+    <row r="97" spans="1:7" ht="14" hidden="1">
       <c r="A97" s="7">
         <v>66490</v>
       </c>
@@ -4137,7 +4147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="13.5" hidden="1">
+    <row r="98" spans="1:7" ht="14" hidden="1">
       <c r="A98" s="7">
         <v>66351</v>
       </c>
@@ -4160,7 +4170,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="13.5" hidden="1">
+    <row r="99" spans="1:7" ht="14" hidden="1">
       <c r="A99" s="7">
         <v>66350</v>
       </c>
@@ -4183,7 +4193,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="13.5" hidden="1">
+    <row r="100" spans="1:7" ht="14" hidden="1">
       <c r="A100" s="7">
         <v>66347</v>
       </c>
@@ -4206,7 +4216,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="13.5" hidden="1">
+    <row r="101" spans="1:7" ht="14" hidden="1">
       <c r="A101" s="7">
         <v>66353</v>
       </c>
@@ -4229,7 +4239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="13.5" hidden="1">
+    <row r="102" spans="1:7" ht="14" hidden="1">
       <c r="A102" s="7">
         <v>66349</v>
       </c>
@@ -4252,7 +4262,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="13.5" hidden="1">
+    <row r="103" spans="1:7" ht="14" hidden="1">
       <c r="A103" s="7">
         <v>66352</v>
       </c>
@@ -4275,7 +4285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="13.5" hidden="1">
+    <row r="104" spans="1:7" ht="14" hidden="1">
       <c r="A104" s="7">
         <v>66488</v>
       </c>
@@ -4298,7 +4308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="13.5" hidden="1">
+    <row r="105" spans="1:7" ht="14" hidden="1">
       <c r="A105" s="7">
         <v>66483</v>
       </c>
@@ -4321,7 +4331,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="13.5" hidden="1">
+    <row r="106" spans="1:7" ht="14" hidden="1">
       <c r="A106" s="7">
         <v>66485</v>
       </c>
@@ -4344,7 +4354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="13.5" hidden="1">
+    <row r="107" spans="1:7" ht="14" hidden="1">
       <c r="A107" s="7">
         <v>66484</v>
       </c>
@@ -4367,7 +4377,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="13.5" hidden="1">
+    <row r="108" spans="1:7" ht="14" hidden="1">
       <c r="A108" s="7">
         <v>66482</v>
       </c>
@@ -4390,7 +4400,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="13.5" hidden="1">
+    <row r="109" spans="1:7" ht="14" hidden="1">
       <c r="A109" s="7">
         <v>66486</v>
       </c>
@@ -4413,7 +4423,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="13.5" hidden="1">
+    <row r="110" spans="1:7" ht="14" hidden="1">
       <c r="A110" s="7">
         <v>66487</v>
       </c>
@@ -4436,7 +4446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="13.5">
+    <row r="111" spans="1:7" ht="14">
       <c r="A111" s="7">
         <v>66458</v>
       </c>
@@ -4459,7 +4469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="13.5">
+    <row r="112" spans="1:7" ht="14">
       <c r="A112" s="7">
         <v>66496</v>
       </c>
@@ -4482,7 +4492,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="13.5">
+    <row r="113" spans="1:7" ht="14">
       <c r="A113" s="7">
         <v>66495</v>
       </c>
@@ -4505,7 +4515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="13.5">
+    <row r="114" spans="1:7" ht="14">
       <c r="A114" s="7">
         <v>66452</v>
       </c>
@@ -4528,7 +4538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="13.5">
+    <row r="115" spans="1:7" ht="14">
       <c r="A115" s="7">
         <v>66492</v>
       </c>
@@ -4551,7 +4561,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="13.5">
+    <row r="116" spans="1:7" ht="14">
       <c r="A116" s="7">
         <v>66493</v>
       </c>
@@ -4574,7 +4584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="13.5">
+    <row r="117" spans="1:7" ht="14">
       <c r="A117" s="7">
         <v>66494</v>
       </c>
@@ -4597,7 +4607,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="13.5">
+    <row r="118" spans="1:7" ht="14">
       <c r="A118" s="7">
         <v>66453</v>
       </c>
@@ -4620,7 +4630,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="13.5" hidden="1">
+    <row r="119" spans="1:7" ht="14" hidden="1">
       <c r="A119" s="7">
         <v>66269</v>
       </c>
@@ -4643,7 +4653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="13.5" hidden="1">
+    <row r="120" spans="1:7" ht="14" hidden="1">
       <c r="A120" s="7">
         <v>66268</v>
       </c>
@@ -4666,7 +4676,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="13.5" hidden="1">
+    <row r="121" spans="1:7" ht="14" hidden="1">
       <c r="A121" s="7">
         <v>66271</v>
       </c>
@@ -4689,7 +4699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="13.5" hidden="1">
+    <row r="122" spans="1:7" ht="14" hidden="1">
       <c r="A122" s="7">
         <v>66267</v>
       </c>
@@ -4712,7 +4722,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="13.5" hidden="1">
+    <row r="123" spans="1:7" ht="14" hidden="1">
       <c r="A123" s="7">
         <v>66650</v>
       </c>
@@ -4735,7 +4745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="13.5" hidden="1">
+    <row r="124" spans="1:7" ht="14" hidden="1">
       <c r="A124" s="7">
         <v>66063</v>
       </c>
@@ -4758,7 +4768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="13.5" hidden="1">
+    <row r="125" spans="1:7" ht="14" hidden="1">
       <c r="A125" s="7">
         <v>66072</v>
       </c>
@@ -4781,7 +4791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="13.5">
+    <row r="126" spans="1:7" ht="14">
       <c r="A126" s="7">
         <v>66727</v>
       </c>
@@ -4804,7 +4814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="13.5">
+    <row r="127" spans="1:7" ht="14">
       <c r="A127" s="7">
         <v>66760</v>
       </c>
@@ -4827,7 +4837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="13.5" hidden="1">
+    <row r="128" spans="1:7" ht="14" hidden="1">
       <c r="A128" s="7">
         <v>66310</v>
       </c>
@@ -4850,7 +4860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="13.5" hidden="1">
+    <row r="129" spans="1:7" ht="14" hidden="1">
       <c r="A129" s="7">
         <v>66291</v>
       </c>
@@ -4873,7 +4883,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="13.5" hidden="1">
+    <row r="130" spans="1:7" ht="14" hidden="1">
       <c r="A130" s="7">
         <v>66297</v>
       </c>
@@ -4896,7 +4906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="13.5" hidden="1">
+    <row r="131" spans="1:7" ht="14" hidden="1">
       <c r="A131" s="7">
         <v>66296</v>
       </c>
@@ -4919,7 +4929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="13.5">
+    <row r="132" spans="1:7" ht="14">
       <c r="A132" s="7">
         <v>66509</v>
       </c>
@@ -4942,7 +4952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="13.5">
+    <row r="133" spans="1:7" ht="14">
       <c r="A133" s="7">
         <v>66510</v>
       </c>
@@ -4965,7 +4975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="13.5">
+    <row r="134" spans="1:7" ht="14">
       <c r="A134" s="7">
         <v>66508</v>
       </c>
@@ -4988,7 +4998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="13.5">
+    <row r="135" spans="1:7" ht="14">
       <c r="A135" s="7">
         <v>66507</v>
       </c>
@@ -5011,7 +5021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="13.5">
+    <row r="136" spans="1:7" ht="14">
       <c r="A136" s="7">
         <v>66467</v>
       </c>
@@ -5034,7 +5044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="13.5">
+    <row r="137" spans="1:7" ht="14">
       <c r="A137" s="7">
         <v>66516</v>
       </c>
@@ -5057,7 +5067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="13.5" hidden="1">
+    <row r="138" spans="1:7" ht="14" hidden="1">
       <c r="A138" s="7">
         <v>66754</v>
       </c>
@@ -5080,7 +5090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="13.5" hidden="1">
+    <row r="139" spans="1:7" ht="14" hidden="1">
       <c r="A139" s="7">
         <v>66091</v>
       </c>
@@ -5103,7 +5113,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="13.5" hidden="1">
+    <row r="140" spans="1:7" ht="14" hidden="1">
       <c r="A140" s="7">
         <v>66081</v>
       </c>
@@ -5126,7 +5136,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="13.5" hidden="1">
+    <row r="141" spans="1:7" ht="14" hidden="1">
       <c r="A141" s="7">
         <v>66096</v>
       </c>
@@ -5149,7 +5159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="13.5" hidden="1">
+    <row r="142" spans="1:7" ht="14" hidden="1">
       <c r="A142" s="7">
         <v>66761</v>
       </c>
@@ -5172,7 +5182,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="13.5" hidden="1">
+    <row r="143" spans="1:7" ht="14" hidden="1">
       <c r="A143" s="7">
         <v>66762</v>
       </c>
@@ -5195,7 +5205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="13.5" hidden="1">
+    <row r="144" spans="1:7" ht="14" hidden="1">
       <c r="A144" s="7">
         <v>66517</v>
       </c>
@@ -5218,7 +5228,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="13.5">
+    <row r="145" spans="1:7" ht="14">
       <c r="A145" s="7">
         <v>66443</v>
       </c>
@@ -5241,7 +5251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="13.5" hidden="1">
+    <row r="146" spans="1:7" ht="14" hidden="1">
       <c r="A146" s="7">
         <v>66098</v>
       </c>
@@ -5264,7 +5274,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="13.5" hidden="1">
+    <row r="147" spans="1:7" ht="14" hidden="1">
       <c r="A147" s="7">
         <v>66097</v>
       </c>
@@ -5287,7 +5297,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="13.5" hidden="1">
+    <row r="148" spans="1:7" ht="14" hidden="1">
       <c r="A148" s="7">
         <v>66071</v>
       </c>
@@ -5310,7 +5320,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="13.5" hidden="1">
+    <row r="149" spans="1:7" ht="14" hidden="1">
       <c r="A149" s="7">
         <v>66069</v>
       </c>
@@ -5333,7 +5343,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="13.5" hidden="1">
+    <row r="150" spans="1:7" ht="14" hidden="1">
       <c r="A150" s="7">
         <v>66070</v>
       </c>
@@ -5356,7 +5366,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="13.5" hidden="1">
+    <row r="151" spans="1:7" ht="14" hidden="1">
       <c r="A151" s="7">
         <v>66745</v>
       </c>
@@ -5379,7 +5389,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="13.5" hidden="1">
+    <row r="152" spans="1:7" ht="14" hidden="1">
       <c r="A152" s="7">
         <v>66060</v>
       </c>
@@ -5402,7 +5412,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="13.5" hidden="1">
+    <row r="153" spans="1:7" ht="14" hidden="1">
       <c r="A153" s="7">
         <v>66048</v>
       </c>
@@ -5425,7 +5435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="13.5" hidden="1">
+    <row r="154" spans="1:7" ht="14" hidden="1">
       <c r="A154" s="7">
         <v>66054</v>
       </c>
@@ -5448,7 +5458,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="13.5" hidden="1">
+    <row r="155" spans="1:7" ht="14" hidden="1">
       <c r="A155" s="7">
         <v>66061</v>
       </c>
@@ -5471,7 +5481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="13.5" hidden="1">
+    <row r="156" spans="1:7" ht="14" hidden="1">
       <c r="A156" s="7">
         <v>66062</v>
       </c>
@@ -5494,7 +5504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="13.5" hidden="1">
+    <row r="157" spans="1:7" ht="14" hidden="1">
       <c r="A157" s="7">
         <v>66088</v>
       </c>
@@ -5517,7 +5527,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="13.5" hidden="1">
+    <row r="158" spans="1:7" ht="14" hidden="1">
       <c r="A158" s="7">
         <v>66085</v>
       </c>
@@ -5540,7 +5550,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="13.5" hidden="1">
+    <row r="159" spans="1:7" ht="14" hidden="1">
       <c r="A159" s="7">
         <v>66086</v>
       </c>
@@ -5563,7 +5573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="13.5" hidden="1">
+    <row r="160" spans="1:7" ht="14" hidden="1">
       <c r="A160" s="7">
         <v>66447</v>
       </c>
@@ -5586,7 +5596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="13.5" hidden="1">
+    <row r="161" spans="1:7" ht="14" hidden="1">
       <c r="A161" s="7">
         <v>66446</v>
       </c>
@@ -5609,7 +5619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="13.5" hidden="1">
+    <row r="162" spans="1:7" ht="14" hidden="1">
       <c r="A162" s="7">
         <v>66376</v>
       </c>
@@ -5632,7 +5642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="13.5" hidden="1">
+    <row r="163" spans="1:7" ht="14" hidden="1">
       <c r="A163" s="7">
         <v>66370</v>
       </c>
@@ -5655,7 +5665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="13.5" hidden="1">
+    <row r="164" spans="1:7" ht="14" hidden="1">
       <c r="A164" s="7">
         <v>66375</v>
       </c>
@@ -5678,7 +5688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="13.5" hidden="1">
+    <row r="165" spans="1:7" ht="14" hidden="1">
       <c r="A165" s="7">
         <v>66272</v>
       </c>
@@ -5701,7 +5711,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="13.5" hidden="1">
+    <row r="166" spans="1:7" ht="14" hidden="1">
       <c r="A166" s="7">
         <v>66273</v>
       </c>
@@ -5724,7 +5734,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="13.5" hidden="1">
+    <row r="167" spans="1:7" ht="14" hidden="1">
       <c r="A167" s="7">
         <v>66275</v>
       </c>
@@ -5747,7 +5757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="13.5" hidden="1">
+    <row r="168" spans="1:7" ht="14" hidden="1">
       <c r="A168" s="7">
         <v>66257</v>
       </c>
@@ -5770,7 +5780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="13.5" hidden="1">
+    <row r="169" spans="1:7" ht="14" hidden="1">
       <c r="A169" s="7">
         <v>66434</v>
       </c>
@@ -5793,7 +5803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="13.5" hidden="1">
+    <row r="170" spans="1:7" ht="14" hidden="1">
       <c r="A170" s="7">
         <v>66302</v>
       </c>
@@ -5816,7 +5826,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="13.5" hidden="1">
+    <row r="171" spans="1:7" ht="14" hidden="1">
       <c r="A171" s="7">
         <v>66528</v>
       </c>
@@ -5839,7 +5849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="13.5" hidden="1">
+    <row r="172" spans="1:7" ht="14" hidden="1">
       <c r="A172" s="7">
         <v>66437</v>
       </c>
@@ -5862,7 +5872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="13.5" hidden="1">
+    <row r="173" spans="1:7" ht="14" hidden="1">
       <c r="A173" s="7">
         <v>66436</v>
       </c>
@@ -5885,7 +5895,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="13.5" hidden="1">
+    <row r="174" spans="1:7" ht="14" hidden="1">
       <c r="A174" s="7">
         <v>66435</v>
       </c>
@@ -5908,7 +5918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="13.5" hidden="1">
+    <row r="175" spans="1:7" ht="14" hidden="1">
       <c r="A175" s="7">
         <v>66286</v>
       </c>
@@ -5931,7 +5941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="13.5" hidden="1">
+    <row r="176" spans="1:7" ht="14" hidden="1">
       <c r="A176" s="7">
         <v>66281</v>
       </c>
@@ -5954,7 +5964,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="13.5" hidden="1">
+    <row r="177" spans="1:7" ht="14" hidden="1">
       <c r="A177" s="7">
         <v>66058</v>
       </c>
@@ -5977,7 +5987,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="13.5" hidden="1">
+    <row r="178" spans="1:7" ht="14" hidden="1">
       <c r="A178" s="7">
         <v>66046</v>
       </c>
@@ -6000,7 +6010,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="13.5" hidden="1">
+    <row r="179" spans="1:7" ht="14" hidden="1">
       <c r="A179" s="7">
         <v>66052</v>
       </c>
@@ -6023,7 +6033,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="13.5" hidden="1">
+    <row r="180" spans="1:7" ht="14" hidden="1">
       <c r="A180" s="7">
         <v>66067</v>
       </c>
@@ -6046,7 +6056,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="13.5" hidden="1">
+    <row r="181" spans="1:7" ht="14" hidden="1">
       <c r="A181" s="7">
         <v>66075</v>
       </c>
@@ -6069,7 +6079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="13.5" hidden="1">
+    <row r="182" spans="1:7" ht="14" hidden="1">
       <c r="A182" s="7">
         <v>66491</v>
       </c>
@@ -6092,7 +6102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="13.5" hidden="1">
+    <row r="183" spans="1:7" ht="14" hidden="1">
       <c r="A183" s="7">
         <v>66394</v>
       </c>
@@ -6115,7 +6125,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="13.5" hidden="1">
+    <row r="184" spans="1:7" ht="14" hidden="1">
       <c r="A184" s="7">
         <v>66359</v>
       </c>
@@ -6138,7 +6148,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="13.5" hidden="1">
+    <row r="185" spans="1:7" ht="14" hidden="1">
       <c r="A185" s="7">
         <v>66361</v>
       </c>
@@ -6161,7 +6171,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="13.5" hidden="1">
+    <row r="186" spans="1:7" ht="14" hidden="1">
       <c r="A186" s="7">
         <v>66360</v>
       </c>
@@ -6184,7 +6194,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="13.5" hidden="1">
+    <row r="187" spans="1:7" ht="14" hidden="1">
       <c r="A187" s="7">
         <v>66348</v>
       </c>
@@ -6207,7 +6217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="13.5" hidden="1">
+    <row r="188" spans="1:7" ht="14" hidden="1">
       <c r="A188" s="7">
         <v>66362</v>
       </c>
@@ -6230,7 +6240,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="13.5" hidden="1">
+    <row r="189" spans="1:7" ht="14" hidden="1">
       <c r="A189" s="7">
         <v>66763</v>
       </c>
@@ -6253,7 +6263,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="13.5" hidden="1">
+    <row r="190" spans="1:7" ht="14" hidden="1">
       <c r="A190" s="7">
         <v>66462</v>
       </c>
@@ -6276,7 +6286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="13.5" hidden="1">
+    <row r="191" spans="1:7" ht="14" hidden="1">
       <c r="A191" s="7">
         <v>66463</v>
       </c>
@@ -6299,7 +6309,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="13.5" hidden="1">
+    <row r="192" spans="1:7" ht="14" hidden="1">
       <c r="A192" s="7">
         <v>66064</v>
       </c>
@@ -6322,7 +6332,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="13.5" hidden="1">
+    <row r="193" spans="1:7" ht="14" hidden="1">
       <c r="A193" s="7">
         <v>66726</v>
       </c>
@@ -6345,7 +6355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="13.5" hidden="1">
+    <row r="194" spans="1:7" ht="14" hidden="1">
       <c r="A194" s="7">
         <v>66448</v>
       </c>
@@ -6368,7 +6378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="13.5" hidden="1">
+    <row r="195" spans="1:7" ht="14" hidden="1">
       <c r="A195" s="7">
         <v>66101</v>
       </c>
@@ -6391,7 +6401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="13.5" hidden="1">
+    <row r="196" spans="1:7" ht="14" hidden="1">
       <c r="A196" s="7">
         <v>66420</v>
       </c>
@@ -6414,7 +6424,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="13.5" hidden="1">
+    <row r="197" spans="1:7" ht="14" hidden="1">
       <c r="A197" s="7">
         <v>66426</v>
       </c>
@@ -6437,7 +6447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="13.5" hidden="1">
+    <row r="198" spans="1:7" ht="14" hidden="1">
       <c r="A198" s="7">
         <v>66418</v>
       </c>
@@ -6460,7 +6470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="13.5" hidden="1">
+    <row r="199" spans="1:7" ht="14" hidden="1">
       <c r="A199" s="7">
         <v>66419</v>
       </c>
@@ -6483,7 +6493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="13.5" hidden="1">
+    <row r="200" spans="1:7" ht="14" hidden="1">
       <c r="A200" s="7">
         <v>66417</v>
       </c>
@@ -6506,7 +6516,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="13.5" hidden="1">
+    <row r="201" spans="1:7" ht="14" hidden="1">
       <c r="A201" s="7">
         <v>66651</v>
       </c>
@@ -6529,7 +6539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="13.5" hidden="1">
+    <row r="202" spans="1:7" ht="14" hidden="1">
       <c r="A202" s="7">
         <v>66295</v>
       </c>
@@ -6552,7 +6562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="13.5" hidden="1">
+    <row r="203" spans="1:7" ht="14" hidden="1">
       <c r="A203" s="7">
         <v>66290</v>
       </c>
@@ -6575,7 +6585,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="13.5" hidden="1">
+    <row r="204" spans="1:7" ht="14" hidden="1">
       <c r="A204" s="7">
         <v>66294</v>
       </c>
@@ -6598,7 +6608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="13.5" hidden="1">
+    <row r="205" spans="1:7" ht="14" hidden="1">
       <c r="A205" s="7">
         <v>66374</v>
       </c>
@@ -6621,7 +6631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="13.5" hidden="1">
+    <row r="206" spans="1:7" ht="14" hidden="1">
       <c r="A206" s="7">
         <v>66372</v>
       </c>
@@ -6644,7 +6654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="207" spans="1:7" ht="13.5" hidden="1">
+    <row r="207" spans="1:7" ht="14" hidden="1">
       <c r="A207" s="7">
         <v>66371</v>
       </c>
@@ -6667,7 +6677,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="13.5" hidden="1">
+    <row r="208" spans="1:7" ht="14" hidden="1">
       <c r="A208" s="7">
         <v>66765</v>
       </c>
@@ -6690,7 +6700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="13.5" hidden="1">
+    <row r="209" spans="1:7" ht="14" hidden="1">
       <c r="A209" s="7">
         <v>66626</v>
       </c>
@@ -6713,7 +6723,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="13.5" hidden="1">
+    <row r="210" spans="1:7" ht="14" hidden="1">
       <c r="A210" s="7">
         <v>66276</v>
       </c>
@@ -6736,7 +6746,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="13.5" hidden="1">
+    <row r="211" spans="1:7" ht="14" hidden="1">
       <c r="A211" s="7">
         <v>66277</v>
       </c>
@@ -6759,7 +6769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="13.5" hidden="1">
+    <row r="212" spans="1:7" ht="14" hidden="1">
       <c r="A212" s="7">
         <v>66356</v>
       </c>
@@ -6782,7 +6792,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="13.5" hidden="1">
+    <row r="213" spans="1:7" ht="14" hidden="1">
       <c r="A213" s="7">
         <v>66355</v>
       </c>
@@ -6805,7 +6815,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="13.5" hidden="1">
+    <row r="214" spans="1:7" ht="14" hidden="1">
       <c r="A214" s="7">
         <v>66278</v>
       </c>
@@ -6828,7 +6838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="13.5" hidden="1">
+    <row r="215" spans="1:7" ht="14" hidden="1">
       <c r="A215" s="7">
         <v>66354</v>
       </c>
@@ -6851,7 +6861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="13.5" hidden="1">
+    <row r="216" spans="1:7" ht="14" hidden="1">
       <c r="A216" s="7">
         <v>66346</v>
       </c>
@@ -6874,7 +6884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="13.5" hidden="1">
+    <row r="217" spans="1:7" ht="14" hidden="1">
       <c r="A217" s="7">
         <v>66358</v>
       </c>
@@ -6897,7 +6907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="13.5" hidden="1">
+    <row r="218" spans="1:7" ht="14" hidden="1">
       <c r="A218" s="7">
         <v>66256</v>
       </c>
@@ -6920,7 +6930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="13.5" hidden="1">
+    <row r="219" spans="1:7" ht="14" hidden="1">
       <c r="A219" s="7">
         <v>66357</v>
       </c>
@@ -6943,7 +6953,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="13.5" hidden="1">
+    <row r="220" spans="1:7" ht="14" hidden="1">
       <c r="A220" s="7">
         <v>66489</v>
       </c>
@@ -6966,7 +6976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="13.5" hidden="1">
+    <row r="221" spans="1:7" ht="14" hidden="1">
       <c r="A221" s="7">
         <v>66764</v>
       </c>
@@ -6989,7 +6999,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="13.5" hidden="1">
+    <row r="222" spans="1:7" ht="14" hidden="1">
       <c r="A222" s="7">
         <v>66505</v>
       </c>
@@ -7012,7 +7022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="13.5" hidden="1">
+    <row r="223" spans="1:7" ht="14" hidden="1">
       <c r="A223" s="7">
         <v>66504</v>
       </c>
@@ -7035,7 +7045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="13.5" hidden="1">
+    <row r="224" spans="1:7" ht="14" hidden="1">
       <c r="A224" s="7">
         <v>66506</v>
       </c>
@@ -7058,7 +7068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="13.5" hidden="1">
+    <row r="225" spans="1:7" ht="14" hidden="1">
       <c r="A225" s="7">
         <v>66503</v>
       </c>
@@ -7081,7 +7091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="13.5" hidden="1">
+    <row r="226" spans="1:7" ht="14" hidden="1">
       <c r="A226" s="7">
         <v>66466</v>
       </c>
@@ -7104,7 +7114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="13.5" hidden="1">
+    <row r="227" spans="1:7" ht="14" hidden="1">
       <c r="A227" s="7">
         <v>66645</v>
       </c>
@@ -7127,7 +7137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="13.5" hidden="1">
+    <row r="228" spans="1:7" ht="14" hidden="1">
       <c r="A228" s="7">
         <v>66649</v>
       </c>
@@ -7150,7 +7160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="13.5" hidden="1">
+    <row r="229" spans="1:7" ht="14" hidden="1">
       <c r="A229" s="7">
         <v>66630</v>
       </c>
@@ -7173,7 +7183,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="230" spans="1:7" ht="13.5" hidden="1">
+    <row r="230" spans="1:7" ht="14" hidden="1">
       <c r="A230" s="7">
         <v>66636</v>
       </c>
@@ -7196,7 +7206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="231" spans="1:7" ht="13.5" hidden="1">
+    <row r="231" spans="1:7" ht="14" hidden="1">
       <c r="A231" s="7">
         <v>66644</v>
       </c>
@@ -7219,7 +7229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="13.5" hidden="1">
+    <row r="232" spans="1:7" ht="14" hidden="1">
       <c r="A232" s="7">
         <v>66047</v>
       </c>
@@ -7242,7 +7252,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="13.5" hidden="1">
+    <row r="233" spans="1:7" ht="14" hidden="1">
       <c r="A233" s="7">
         <v>66053</v>
       </c>
@@ -7265,7 +7275,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="13.5" hidden="1">
+    <row r="234" spans="1:7" ht="14" hidden="1">
       <c r="A234" s="7">
         <v>66059</v>
       </c>
@@ -7288,7 +7298,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="235" spans="1:7" ht="13.5" hidden="1">
+    <row r="235" spans="1:7" ht="14" hidden="1">
       <c r="A235" s="7">
         <v>66057</v>
       </c>
@@ -7311,7 +7321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="13.5" hidden="1">
+    <row r="236" spans="1:7" ht="14" hidden="1">
       <c r="A236" s="7">
         <v>66045</v>
       </c>
@@ -7334,7 +7344,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="13.5" hidden="1">
+    <row r="237" spans="1:7" ht="14" hidden="1">
       <c r="A237" s="7">
         <v>66051</v>
       </c>
@@ -7357,7 +7367,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="238" spans="1:7" ht="13.5" hidden="1">
+    <row r="238" spans="1:7" ht="14" hidden="1">
       <c r="A238" s="7">
         <v>66299</v>
       </c>
@@ -7380,7 +7390,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="13.5" hidden="1">
+    <row r="239" spans="1:7" ht="14" hidden="1">
       <c r="A239" s="7">
         <v>66432</v>
       </c>
@@ -7403,7 +7413,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="13.5" hidden="1">
+    <row r="240" spans="1:7" ht="14" hidden="1">
       <c r="A240" s="7">
         <v>66300</v>
       </c>
@@ -7426,7 +7436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="13.5" hidden="1">
+    <row r="241" spans="1:7" ht="14" hidden="1">
       <c r="A241" s="7">
         <v>66634</v>
       </c>
@@ -7449,7 +7459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="13.5" hidden="1">
+    <row r="242" spans="1:7" ht="14" hidden="1">
       <c r="A242" s="7">
         <v>66652</v>
       </c>
@@ -7472,7 +7482,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="13.5" hidden="1">
+    <row r="243" spans="1:7" ht="14" hidden="1">
       <c r="A243" s="7">
         <v>66639</v>
       </c>
@@ -7495,7 +7505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="244" spans="1:7" ht="13.5" hidden="1">
+    <row r="244" spans="1:7" ht="14" hidden="1">
       <c r="A244" s="7">
         <v>66314</v>
       </c>
@@ -7518,7 +7528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="13.5" hidden="1">
+    <row r="245" spans="1:7" ht="14" hidden="1">
       <c r="A245" s="7">
         <v>66387</v>
       </c>
@@ -7541,7 +7551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="13.5" hidden="1">
+    <row r="246" spans="1:7" ht="14" hidden="1">
       <c r="A246" s="7">
         <v>66385</v>
       </c>
@@ -7564,7 +7574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="13.5" hidden="1">
+    <row r="247" spans="1:7" ht="14" hidden="1">
       <c r="A247" s="7">
         <v>66382</v>
       </c>
@@ -7587,7 +7597,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="248" spans="1:7" ht="13.5" hidden="1">
+    <row r="248" spans="1:7" ht="14" hidden="1">
       <c r="A248" s="7">
         <v>66383</v>
       </c>
@@ -7610,7 +7620,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="13.5" hidden="1">
+    <row r="249" spans="1:7" ht="14" hidden="1">
       <c r="A249" s="7">
         <v>66384</v>
       </c>
@@ -7633,7 +7643,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="13.5" hidden="1">
+    <row r="250" spans="1:7" ht="14" hidden="1">
       <c r="A250" s="7">
         <v>66633</v>
       </c>
@@ -7656,7 +7666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="13.5" hidden="1">
+    <row r="251" spans="1:7" ht="14" hidden="1">
       <c r="A251" s="7">
         <v>66647</v>
       </c>
@@ -7679,7 +7689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="13.5" hidden="1">
+    <row r="252" spans="1:7" ht="14" hidden="1">
       <c r="A252" s="7">
         <v>66526</v>
       </c>
@@ -7702,7 +7712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="253" spans="1:7" ht="13.5" hidden="1">
+    <row r="253" spans="1:7" ht="14" hidden="1">
       <c r="A253" s="7">
         <v>66524</v>
       </c>
@@ -7725,7 +7735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="254" spans="1:7" ht="13.5" hidden="1">
+    <row r="254" spans="1:7" ht="14" hidden="1">
       <c r="A254" s="7">
         <v>66513</v>
       </c>
@@ -7748,7 +7758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="13.5" hidden="1">
+    <row r="255" spans="1:7" ht="14" hidden="1">
       <c r="A255" s="7">
         <v>66512</v>
       </c>
@@ -7771,7 +7781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="13.5" hidden="1">
+    <row r="256" spans="1:7" ht="14" hidden="1">
       <c r="A256" s="7">
         <v>66514</v>
       </c>
@@ -7794,7 +7804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="257" spans="1:7" ht="13.5" hidden="1">
+    <row r="257" spans="1:7" ht="14" hidden="1">
       <c r="A257" s="7">
         <v>66511</v>
       </c>
@@ -7817,7 +7827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="258" spans="1:7" ht="13.5" hidden="1">
+    <row r="258" spans="1:7" ht="14" hidden="1">
       <c r="A258" s="7">
         <v>66755</v>
       </c>
@@ -7840,7 +7850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="259" spans="1:7" ht="13.5">
+    <row r="259" spans="1:7" ht="14">
       <c r="A259" s="7">
         <v>66766</v>
       </c>
@@ -7863,7 +7873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260" spans="1:7" ht="13.5" hidden="1">
+    <row r="260" spans="1:7" ht="14" hidden="1">
       <c r="A260" s="7">
         <v>66094</v>
       </c>
@@ -7886,7 +7896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="1:7" ht="13.5" hidden="1">
+    <row r="261" spans="1:7" ht="14" hidden="1">
       <c r="A261" s="7">
         <v>66431</v>
       </c>
@@ -7909,7 +7919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="262" spans="1:7" ht="13.5" hidden="1">
+    <row r="262" spans="1:7" ht="14" hidden="1">
       <c r="A262" s="7">
         <v>66430</v>
       </c>
@@ -7932,7 +7942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263" spans="1:7" ht="13.5" hidden="1">
+    <row r="263" spans="1:7" ht="14" hidden="1">
       <c r="A263" s="7">
         <v>66767</v>
       </c>
@@ -7955,7 +7965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="264" spans="1:7" ht="13.5" hidden="1">
+    <row r="264" spans="1:7" ht="14" hidden="1">
       <c r="A264" s="7">
         <v>66653</v>
       </c>
@@ -7978,7 +7988,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265" spans="1:7" ht="13.5" hidden="1">
+    <row r="265" spans="1:7" ht="14" hidden="1">
       <c r="A265" s="7">
         <v>66100</v>
       </c>
@@ -8001,7 +8011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="266" spans="1:7" ht="13.5" hidden="1">
+    <row r="266" spans="1:7" ht="14" hidden="1">
       <c r="A266" s="7">
         <v>66768</v>
       </c>
@@ -8027,7 +8037,7 @@
     <row r="269" spans="1:7">
       <c r="G269" s="3"/>
     </row>
-    <row r="271" spans="1:7" ht="13.5">
+    <row r="271" spans="1:7">
       <c r="A271" s="4"/>
       <c r="F271" s="13"/>
       <c r="G271" s="5"/>
@@ -8057,6 +8067,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="7f019ab0-5ffe-43e1-b2f8-62bc369ebe4f" xsi:nil="true"/>
@@ -8065,15 +8084,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8332,13 +8342,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A058DE5-6E99-4129-8DC4-E9679F94EDB3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072A20B5-EC58-4873-ACA8-86FA21EFF473}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072A20B5-EC58-4873-ACA8-86FA21EFF473}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A058DE5-6E99-4129-8DC4-E9679F94EDB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7f019ab0-5ffe-43e1-b2f8-62bc369ebe4f"/>
+    <ds:schemaRef ds:uri="95c80e47-662b-4bc0-a457-b879d3f3aba4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4F0E0D1-DD0C-4933-B42A-72A4BE23F218}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4F0E0D1-DD0C-4933-B42A-72A4BE23F218}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="95c80e47-662b-4bc0-a457-b879d3f3aba4"/>
+    <ds:schemaRef ds:uri="7f019ab0-5ffe-43e1-b2f8-62bc369ebe4f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>